<commit_message>
fixes #2382, #2414, #2416, #2412, changes discussed on 2023-07-28
</commit_message>
<xml_diff>
--- a/data/translations.04_ra.xlsx
+++ b/data/translations.04_ra.xlsx
@@ -121,13 +121,13 @@
     <t xml:space="preserve">ref_dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">citation reference for dataset</t>
+    <t xml:space="preserve">cite the dataset</t>
   </si>
   <si>
     <t xml:space="preserve">ref_entry</t>
   </si>
   <si>
-    <t xml:space="preserve">citation reference for this data entry</t>
+    <t xml:space="preserve">cite this entry</t>
   </si>
   <si>
     <t xml:space="preserve">contact</t>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -339,7 +339,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Sofya issues by mail on 2023-08-03
</commit_message>
<xml_diff>
--- a/data/translations.04_ra.xlsx
+++ b/data/translations.04_ra.xlsx
@@ -339,7 +339,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -616,7 +616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
adds dataset download button
</commit_message>
<xml_diff>
--- a/data/translations.04_ra.xlsx
+++ b/data/translations.04_ra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t xml:space="preserve">Royal Academy of Painting and Sculpture, reception pieces, Louvre, eighteenth-century French art, seventeenth-century French art, eighteenth century art France, seventeenth century art France, eighteenth century painting, seventeenth century painting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">download_dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">télécharger l'ensemble de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">download the complete dataset</t>
   </si>
 </sst>
 </file>
@@ -430,15 +439,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,12 +641,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1225,6 +1234,17 @@
         <v>108</v>
       </c>
     </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixes single view button tooltips
</commit_message>
<xml_diff>
--- a/data/translations.04_ra.xlsx
+++ b/data/translations.04_ra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -356,6 +356,42 @@
   </si>
   <si>
     <t xml:space="preserve">download the complete dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print_entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imprimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print this entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">données JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_to_watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter à la watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add to watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove_from_watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer de la watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove from watchlist</t>
   </si>
 </sst>
 </file>
@@ -641,12 +677,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+      <selection pane="bottomLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1245,6 +1281,50 @@
         <v>111</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixes issues reported by mail
</commit_message>
<xml_diff>
--- a/data/translations.04_ra.xlsx
+++ b/data/translations.04_ra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="157">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -394,13 +394,205 @@
     <t xml:space="preserve">remove from watchlist</t>
   </si>
   <si>
-    <t xml:space="preserve">map_source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source d'image : Bibliothèque de l'Institut national d'histoire de l'art, collections Jacques Doucet, 12 RES 870, crédit photo — INHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image source: Bibliothèque de l'Institut national d'histoire de l'art, collections Jacques Doucet, 12 RES 870, photo credit — INHA</t>
+    <t xml:space="preserve">map_cite_this_page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citer cette page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cite this page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_cite_this_page_text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Castor, Markus A., Anne Klammt, and Sofya Dmitrieva (eds.), “Académie Royale Art Collection Database. %{room_label},” DFK Paris. August 31, 2023. URL: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.dfk-paris.org/fr/page/academie-database-3846.html#/maps/%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{room_id}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Castor, Markus A., Anne Klammt, and Sofya Dmitrieva (eds.), “Académie Royale Art Collection Database. %{room_label},” DFK Paris. August 31, 2023. URL: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.dfk-paris.org/en/page/academie-database-3846.html#/maps/%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{room_id}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">map_cite_the_dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citer l'ensemble de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cite the dataset</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">map_cite_the_dataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_text</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Castor, Markus A., Anne Klammt, and Sofya Dmitrieva (eds.), “Académie Royale Art Collection Database,” DFK Paris. August 31, 2023. URL: https://www.dfk-paris.org/fr/page/academie-database-3846.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castor, Markus A., Anne Klammt, and Sofya Dmitrieva (eds.), “Académie Royale Art Collection Database,” DFK Paris. August 31, 2023. URL: https://www.dfk-paris.org/en/page/academie-database-3846.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous contacter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">map_contact</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_text</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">This page* is the result of ongoing research. We would be happy to improve or correct it. If you are aware of additional information or inconsistencies, please contact us at collection-academieroyale@dfk-paris.org.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'utilisation des données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">map_use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_text</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">La présente page est le résultat du travail du DFK Paris et peut être utilisée librement. Les plans originaux tirés de l'inventaire de Nicolas Guérin nous ont été aimablement fournis par l'INHA et sont soumis au droit d'auteur (source de l'image : Bibliothèque de l'Institut national d'histoire de l'art, collections Jacques Doucet, 12 RES 870 ; crédit photo : INHA).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The present page is the result of the intellectual work of the DFK Paris and can be used freely. The original plans from Nicolas Guérin's inventory were kindly provided to us by the INHA and are subject to copyright (image source: Bibliothèque de l'Institut national d'histoire de l'art, collections Jacques Doucet, 12 RES 870; photo credit: INHA).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_name_salon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_name_salle-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troisième salle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_name_salle-assemblee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salle d'Assemblée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_name_salle-separee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salle separée des autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_name_vestibule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vestibule</t>
   </si>
 </sst>
 </file>
@@ -410,7 +602,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -431,6 +623,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -479,7 +683,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,6 +701,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,12 +898,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="bottomLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1338,7 +1546,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>124</v>
       </c>
@@ -1349,7 +1557,143 @@
         <v>126</v>
       </c>
     </row>
+    <row r="55" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C55" r:id="rId1" location="/maps/%25" display="https://www.dfk-paris.org/fr/page/academie-database-3846.html#/maps/%"/>
+    <hyperlink ref="D55" r:id="rId2" location="/maps/%25" display="https://www.dfk-paris.org/en/page/academie-database-3846.html#/maps/%"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>